<commit_message>
corecting additional variable names
</commit_message>
<xml_diff>
--- a/data_processing_elements-KSA.xlsx
+++ b/data_processing_elements-KSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\Boulot\ProPASS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87A871F-BEFC-49B5-A992-D8E8138E45C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E9A127-8F5E-44DC-90C0-D82732DDA5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{61CF0716-E47C-4322-AF00-25CE3B72351E}"/>
   </bookViews>
@@ -1490,8 +1490,126 @@
     <t>Work_status</t>
   </si>
   <si>
+    <t>Occupational_Code</t>
+  </si>
+  <si>
+    <t>Work_time</t>
+  </si>
+  <si>
+    <t>ifelse(is.na(WC), NA, 2)</t>
+  </si>
+  <si>
+    <t>Last_time_had_food</t>
+  </si>
+  <si>
+    <t>case_when(
+hour(hm(Last_time_had_food)) + minute(hm(Last_time_had_food)) / 60 &gt; 4 ~ 2L;
+hour(hm(Last_time_had_food)) + minute(hm(Last_time_had_food)) / 60 &lt;= 4 &amp; hour(hm(Last_time_had_food)) + minute(hm(Last_time_had_food)) / 60 &gt; 0 ~ 1L;
+hour(hm(Last_time_had_food)) + minute(hm(Last_time_had_food)) / 60 == 0 ~ 0L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>HDL_CHOL</t>
+  </si>
+  <si>
+    <t>CHOL/38.67</t>
+  </si>
+  <si>
+    <t>HDL_CHOL/38.67</t>
+  </si>
+  <si>
+    <t>TRIG/88.57</t>
+  </si>
+  <si>
+    <t>LDL_CALC</t>
+  </si>
+  <si>
+    <t>N_Cigarettes_Day</t>
+  </si>
+  <si>
+    <t>N_Cigarettes_Day/7</t>
+  </si>
+  <si>
+    <t>Health_Perception</t>
+  </si>
+  <si>
+    <t>CHS_Diabetes</t>
+  </si>
+  <si>
+    <t>CHS_Cancer</t>
+  </si>
+  <si>
+    <t>HSP_Cholesterol</t>
+  </si>
+  <si>
+    <t>HSP_Glucose</t>
+  </si>
+  <si>
+    <t>HSP_Hypertension</t>
+  </si>
+  <si>
+    <t>CHS_Mental_health</t>
+  </si>
+  <si>
+    <t>PSQI_Hour_of_sleep_pe_night</t>
+  </si>
+  <si>
+    <t>hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60</t>
+  </si>
+  <si>
+    <t>case_when(
+hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt;= 0 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 6.25 ~ 1L;
+hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 6.25 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 6.75 ~ 2L;
+hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 6.75 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 7.25 ~ 3L;
+hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 7.25 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 7.75 ~ 4L;
+hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 7.75 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 8.25 ~ 5L;
+hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 8.25 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 8.75 ~ 6L;
+hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 8.75 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 9.25 ~ 7L;
+hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 9.25 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 9.75 ~ 8L;
+hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt;= 10 ~ 9L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+GPAQ_at_work_vigorous_intensity_activity == 1 |
+GPAQ_at_work_moderate_intensity_activity == 1 ~ 1L;
+GPAQ_at_work_vigorous_intensity_activity == 0 &amp;
+GPAQ_at_work_moderate_intensity_activity == 0 ~ 0L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>GPAQ_at_work_vigorous_intensity_activity;
+GPAQ_at_work_moderate_intensity_activity</t>
+  </si>
+  <si>
+    <t>CHS_Arthritis;
+CHS_Bechterews_disease;
+CHS_Osteoporosis;
+CHS_Arthrosis</t>
+  </si>
+  <si>
+    <t>case_when(
+CHS_Arthritis == 1 |
+CHS_Bechterews_disease == 1 |
+CHS_Arthrosis == 1 |
+CHS_Osteoporosis == 1 ~ 1L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>rowSums(mutate(.,
+phq9_1 = (PHQ9_Little interest - 1),
+phq9_2 = (PHQ9_Feeling_down - 1), 
+phq9_3 = (PHQ9_Trouble_falling - 1),
+phq9_4 = (PHQ9_Feeling_tired - 1),
+phq9_5 = (PHQ9_Poor_appetite - 1),
+phq9_6 = (PHQ9_Feeling_bad_about_yourself - 1),
+phq9_7 = (PHQ9_Trouble_concentrating - 1),
+phq9_8 = (PHQ9_Moving_or_speaking - 1),
+phq9_9 = (PHQ9_Thoughts_that_you - 1)) %&gt;% select(phq9_1 , phq9_2 , phq9_3 , phq9_4 , phq9_5 , phq9_6 , phq9_7 , phq9_8 , phq9_9), na.rm = TRUE)</t>
+  </si>
+  <si>
     <t>case_when( 
-Occupational_Main_Code == 0 ~ "Not working due to retirement or other reasons related to employment status"; 
+Occupational_Code == 0 ~ "Not working due to retirement or other reasons related to employment status"; 
 Occupational_Code == 1 ~ "Manager"; 
 Occupational_Code == 2 ~ "Specialist"; 
 Occupational_Code == 3 ~ "Technicians and associate professionals"; 
@@ -1505,54 +1623,11 @@
 ELSE ~ NA_character_)</t>
   </si>
   <si>
-    <t>Occupational_Code</t>
-  </si>
-  <si>
-    <t>Work_time</t>
-  </si>
-  <si>
-    <t>ifelse(is.na(WC), NA, 2)</t>
-  </si>
-  <si>
-    <t>Last_time_had_food</t>
-  </si>
-  <si>
-    <t>case_when(
-hour(hm(Last_time_had_food)) + minute(hm(Last_time_had_food)) / 60 &gt; 4 ~ 2L;
-hour(hm(Last_time_had_food)) + minute(hm(Last_time_had_food)) / 60 &lt;= 4 &amp; hour(hm(Last_time_had_food)) + minute(hm(Last_time_had_food)) / 60 &gt; 0 ~ 1L;
-hour(hm(Last_time_had_food)) + minute(hm(Last_time_had_food)) / 60 == 0 ~ 0L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>HDL_CHOL</t>
-  </si>
-  <si>
-    <t>CHOL/38.67</t>
-  </si>
-  <si>
-    <t>HDL_CHOL/38.67</t>
-  </si>
-  <si>
-    <t>TRIG/88.57</t>
-  </si>
-  <si>
-    <t>LDL_CALC</t>
-  </si>
-  <si>
-    <t>N_Cigarettes_Day</t>
-  </si>
-  <si>
-    <t>N_Cigarettes_Day/7</t>
-  </si>
-  <si>
-    <t>Health_Perception</t>
-  </si>
-  <si>
     <t>CHS_Angina;
 CHS_Myocardial_infarction;
 CHS_Heart_failure;
 CHS_Atrial_fibrillation;
-CHS_Stroke/brain;
+CHS_Stroke_brain;
 CHS_Thrombosis;
 CHS_Peripheral_vascular</t>
   </si>
@@ -1562,85 +1637,10 @@
 CHS_Myocardial_infarction == 1 |
 CHS_Heart_failure == 1 |
 CHS_Atrial_fibrillation == 1 |
-CHS_Stroke/brain == 1 |
+CHS_Stroke_brain == 1 |
 CHS_Thrombosis == 1 |
 CHS_Peripheral_vascular == 1 ~ 1L;
 ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>CHS_Diabetes</t>
-  </si>
-  <si>
-    <t>CHS_Cancer</t>
-  </si>
-  <si>
-    <t>HSP_Cholesterol</t>
-  </si>
-  <si>
-    <t>HSP_Glucose</t>
-  </si>
-  <si>
-    <t>HSP_Hypertension</t>
-  </si>
-  <si>
-    <t>CHS_Mental_health</t>
-  </si>
-  <si>
-    <t>PSQI_Hour_of_sleep_pe_night</t>
-  </si>
-  <si>
-    <t>hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60</t>
-  </si>
-  <si>
-    <t>case_when(
-hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt;= 0 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 6.25 ~ 1L;
-hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 6.25 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 6.75 ~ 2L;
-hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 6.75 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 7.25 ~ 3L;
-hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 7.25 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 7.75 ~ 4L;
-hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 7.75 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 8.25 ~ 5L;
-hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 8.25 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 8.75 ~ 6L;
-hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 8.75 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 9.25 ~ 7L;
-hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt; 9.25 &amp; hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &lt;= 9.75 ~ 8L;
-hour(hm(PSQI_Hour_of_sleep_pe_night)) + minute(hm(PSQI_Hour_of_sleep_pe_night)) / 60 &gt;= 10 ~ 9L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(
-GPAQ_at_work_vigorous_intensity_activity == 1 |
-GPAQ_at_work_moderate_intensity_activity == 1 ~ 1L;
-GPAQ_at_work_vigorous_intensity_activity == 0 &amp;
-GPAQ_at_work_moderate_intensity_activity == 0 ~ 0L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>GPAQ_at_work_vigorous_intensity_activity;
-GPAQ_at_work_moderate_intensity_activity</t>
-  </si>
-  <si>
-    <t>CHS_Arthritis;
-CHS_Bechterews_disease;
-CHS_Osteoporosis;
-CHS_Arthrosis</t>
-  </si>
-  <si>
-    <t>case_when(
-CHS_Arthritis == 1 |
-CHS_Bechterews_disease == 1 |
-CHS_Arthrosis == 1 |
-CHS_Osteoporosis == 1 ~ 1L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>rowSums(mutate(.,
-phq9_1 = (PHQ9_Little interest - 1),
-phq9_2 = (PHQ9_Feeling_down - 1), 
-phq9_3 = (PHQ9_Trouble_falling - 1),
-phq9_4 = (PHQ9_Feeling_tired - 1),
-phq9_5 = (PHQ9_Poor_appetite - 1),
-phq9_6 = (PHQ9_Feeling_bad_about_yourself - 1),
-phq9_7 = (PHQ9_Trouble_concentrating - 1),
-phq9_8 = (PHQ9_Moving_or_speaking - 1),
-phq9_9 = (PHQ9_Thoughts_that_you - 1)) %&gt;% select(phq9_1 , phq9_2 , phq9_3 , phq9_4 , phq9_5 , phq9_6 , phq9_7 , phq9_8 , phq9_9), na.rm = TRUE)</t>
   </si>
 </sst>
 </file>
@@ -2017,12 +2017,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95823C6-700A-48B1-B043-8AB16BFC9FF7}">
   <dimension ref="A1:W84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J53" workbookViewId="0">
-      <selection activeCell="W63" sqref="W63"/>
+    <sheetView tabSelected="1" topLeftCell="I50" workbookViewId="0">
+      <selection activeCell="S63" sqref="S63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="43" customWidth="1"/>
     <col min="9" max="9" width="76.42578125" customWidth="1"/>
     <col min="10" max="10" width="34.85546875" customWidth="1"/>
     <col min="17" max="17" width="69.28515625" customWidth="1"/>
@@ -2425,7 +2426,7 @@
         <v>81</v>
       </c>
       <c r="J9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K9" t="s">
         <v>82</v>
@@ -2501,7 +2502,7 @@
         <v>27</v>
       </c>
       <c r="J11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K11" t="s">
         <v>94</v>
@@ -2519,7 +2520,7 @@
         <v>96</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>376</v>
+        <v>403</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="180" x14ac:dyDescent="0.25">
@@ -2997,7 +2998,7 @@
         <v>43</v>
       </c>
       <c r="W22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -3275,7 +3276,7 @@
         <v>171</v>
       </c>
       <c r="J29" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K29" t="s">
         <v>172</v>
@@ -3296,7 +3297,7 @@
         <v>96</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
@@ -3422,7 +3423,7 @@
         <v>43</v>
       </c>
       <c r="W32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -3448,7 +3449,7 @@
         <v>183</v>
       </c>
       <c r="J33" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K33" t="s">
         <v>188</v>
@@ -3472,7 +3473,7 @@
         <v>43</v>
       </c>
       <c r="W33" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
@@ -3536,7 +3537,7 @@
         <v>183</v>
       </c>
       <c r="J35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K35" t="s">
         <v>193</v>
@@ -3610,7 +3611,7 @@
         <v>51</v>
       </c>
       <c r="W36" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -4034,7 +4035,7 @@
         <v>239</v>
       </c>
       <c r="J47" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K47" t="s">
         <v>240</v>
@@ -4052,7 +4053,7 @@
         <v>43</v>
       </c>
       <c r="W47" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="48" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -4078,7 +4079,7 @@
         <v>243</v>
       </c>
       <c r="J48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K48" t="s">
         <v>244</v>
@@ -4099,7 +4100,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="225" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" ht="135" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4122,7 +4123,7 @@
         <v>250</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="Q49" s="1" t="s">
         <v>251</v>
@@ -4140,7 +4141,7 @@
         <v>96</v>
       </c>
       <c r="W49" s="1" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
     </row>
     <row r="50" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -4166,7 +4167,7 @@
         <v>250</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="S50" t="s">
         <v>256</v>
@@ -4181,7 +4182,7 @@
         <v>96</v>
       </c>
       <c r="W50" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="51" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -4207,7 +4208,7 @@
         <v>250</v>
       </c>
       <c r="J51" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="K51" t="s">
         <v>258</v>
@@ -4289,7 +4290,7 @@
         <v>250</v>
       </c>
       <c r="J53" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="K53" t="s">
         <v>265</v>
@@ -4371,7 +4372,7 @@
         <v>250</v>
       </c>
       <c r="J55" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="K55" t="s">
         <v>271</v>
@@ -4415,7 +4416,7 @@
         <v>250</v>
       </c>
       <c r="J56" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="K56" t="s">
         <v>274</v>
@@ -4459,7 +4460,7 @@
         <v>250</v>
       </c>
       <c r="J57" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="K57" t="s">
         <v>277</v>
@@ -4503,7 +4504,7 @@
         <v>250</v>
       </c>
       <c r="J58" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="K58" t="s">
         <v>281</v>
@@ -4696,7 +4697,7 @@
         <v>43</v>
       </c>
       <c r="W63" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
@@ -4830,7 +4831,7 @@
         <v>302</v>
       </c>
       <c r="J67" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="K67" t="s">
         <v>303</v>
@@ -4851,7 +4852,7 @@
         <v>96</v>
       </c>
       <c r="W67" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="68" spans="1:23" ht="405" x14ac:dyDescent="0.25">
@@ -4877,7 +4878,7 @@
         <v>306</v>
       </c>
       <c r="J68" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="K68" t="s">
         <v>303</v>
@@ -4898,7 +4899,7 @@
         <v>96</v>
       </c>
       <c r="W68" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="69" spans="1:23" ht="75" x14ac:dyDescent="0.25">
@@ -5308,7 +5309,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:23" ht="120" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5448,7 +5449,7 @@
         <v>250</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="Q82" s="1" t="s">
         <v>364</v>
@@ -5463,7 +5464,7 @@
         <v>96</v>
       </c>
       <c r="W82" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
correcting cigarettes variable and lab
</commit_message>
<xml_diff>
--- a/data_processing_elements-KSA.xlsx
+++ b/data_processing_elements-KSA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\Boulot\ProPASS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C925B62A-57E8-47E0-8134-47971F700EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D740D591-3870-4BDF-A341-ABA9F762885B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{61CF0716-E47C-4322-AF00-25CE3B72351E}"/>
   </bookViews>
@@ -1497,22 +1497,10 @@
     <t>HDL_CHOL</t>
   </si>
   <si>
-    <t>CHOL/38.67</t>
-  </si>
-  <si>
-    <t>HDL_CHOL/38.67</t>
-  </si>
-  <si>
-    <t>TRIG/88.57</t>
-  </si>
-  <si>
     <t>LDL_CALC</t>
   </si>
   <si>
     <t>N_Cigarettes_Day</t>
-  </si>
-  <si>
-    <t>N_Cigarettes_Day/7</t>
   </si>
   <si>
     <t>Health_Perception</t>
@@ -1642,6 +1630,18 @@
 PHQ9_Moving_or_speaking;
 PHQ9_Thoughts_that_you
 </t>
+  </si>
+  <si>
+    <t>as.numeric(N_Cigarettes_Day)/7</t>
+  </si>
+  <si>
+    <t>as.numeric(TRIG)/88.57</t>
+  </si>
+  <si>
+    <t>as.numeric(HDL_CHOL)/38.67</t>
+  </si>
+  <si>
+    <t>as.numeric(CHOL)/38.67</t>
   </si>
 </sst>
 </file>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95823C6-700A-48B1-B043-8AB16BFC9FF7}">
   <dimension ref="A1:W84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J54" workbookViewId="0">
-      <selection activeCell="O63" sqref="O63"/>
+    <sheetView tabSelected="1" topLeftCell="J16" workbookViewId="0">
+      <selection activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2503,7 +2503,7 @@
         <v>27</v>
       </c>
       <c r="J11" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="K11" t="s">
         <v>94</v>
@@ -2521,7 +2521,7 @@
         <v>96</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="180" x14ac:dyDescent="0.25">
@@ -3424,7 +3424,7 @@
         <v>43</v>
       </c>
       <c r="W32" t="s">
-        <v>380</v>
+        <v>405</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -3474,7 +3474,7 @@
         <v>43</v>
       </c>
       <c r="W33" t="s">
-        <v>381</v>
+        <v>404</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
@@ -3538,7 +3538,7 @@
         <v>183</v>
       </c>
       <c r="J35" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="K35" t="s">
         <v>193</v>
@@ -3612,7 +3612,7 @@
         <v>51</v>
       </c>
       <c r="W36" t="s">
-        <v>382</v>
+        <v>403</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -4036,7 +4036,7 @@
         <v>239</v>
       </c>
       <c r="J47" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="K47" t="s">
         <v>240</v>
@@ -4054,7 +4054,7 @@
         <v>43</v>
       </c>
       <c r="W47" t="s">
-        <v>385</v>
+        <v>402</v>
       </c>
     </row>
     <row r="48" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -4080,7 +4080,7 @@
         <v>243</v>
       </c>
       <c r="J48" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="K48" t="s">
         <v>244</v>
@@ -4124,7 +4124,7 @@
         <v>250</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="Q49" s="1" t="s">
         <v>251</v>
@@ -4142,7 +4142,7 @@
         <v>96</v>
       </c>
       <c r="W49" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="50" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -4168,7 +4168,7 @@
         <v>250</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="S50" t="s">
         <v>256</v>
@@ -4183,7 +4183,7 @@
         <v>96</v>
       </c>
       <c r="W50" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="51" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -4209,7 +4209,7 @@
         <v>250</v>
       </c>
       <c r="J51" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="K51" t="s">
         <v>258</v>
@@ -4291,7 +4291,7 @@
         <v>250</v>
       </c>
       <c r="J53" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="K53" t="s">
         <v>265</v>
@@ -4373,7 +4373,7 @@
         <v>250</v>
       </c>
       <c r="J55" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="K55" t="s">
         <v>271</v>
@@ -4417,7 +4417,7 @@
         <v>250</v>
       </c>
       <c r="J56" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="K56" t="s">
         <v>274</v>
@@ -4461,7 +4461,7 @@
         <v>250</v>
       </c>
       <c r="J57" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="K57" t="s">
         <v>277</v>
@@ -4505,7 +4505,7 @@
         <v>250</v>
       </c>
       <c r="J58" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="K58" t="s">
         <v>281</v>
@@ -4686,7 +4686,7 @@
         <v>48</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="T63" t="s">
         <v>32</v>
@@ -4698,7 +4698,7 @@
         <v>43</v>
       </c>
       <c r="W63" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
@@ -4832,7 +4832,7 @@
         <v>301</v>
       </c>
       <c r="J67" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="K67" t="s">
         <v>302</v>
@@ -4853,7 +4853,7 @@
         <v>96</v>
       </c>
       <c r="W67" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="68" spans="1:23" ht="405" x14ac:dyDescent="0.25">
@@ -4879,7 +4879,7 @@
         <v>305</v>
       </c>
       <c r="J68" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="K68" t="s">
         <v>302</v>
@@ -4900,7 +4900,7 @@
         <v>96</v>
       </c>
       <c r="W68" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="69" spans="1:23" ht="75" x14ac:dyDescent="0.25">
@@ -5450,7 +5450,7 @@
         <v>250</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="Q82" s="1" t="s">
         <v>363</v>
@@ -5465,7 +5465,7 @@
         <v>96</v>
       </c>
       <c r="W82" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>